<commit_message>
new concepts and categories
</commit_message>
<xml_diff>
--- a/omop-questionconceptid-script/SCD_JobPackage.xlsx
+++ b/omop-questionconceptid-script/SCD_JobPackage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4913,7 +4913,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>2000000156</v>
+        <v>2000000154</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -4946,7 +4946,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>2000000157</v>
+        <v>2000000155</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -4979,7 +4979,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>2000000158</v>
+        <v>2000000156</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>2000000159</v>
+        <v>2000000157</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -5045,7 +5045,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>2000000160</v>
+        <v>2000000158</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -5078,7 +5078,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>2000000161</v>
+        <v>2000000159</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -5111,7 +5111,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>2000000162</v>
+        <v>2000000160</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -5144,7 +5144,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>2000000163</v>
+        <v>2000000161</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -5177,7 +5177,7 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>2000000164</v>
+        <v>2000000162</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -5210,7 +5210,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>2000000170</v>
+        <v>2000000163</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -5243,7 +5243,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>2000000171</v>
+        <v>2000000164</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -5276,7 +5276,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>2000000172</v>
+        <v>2000000165</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -5309,14 +5309,410 @@
         </is>
       </c>
       <c r="E149" t="n">
+        <v>2000000166</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Primary Treatment</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>2000000167</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>First Sickle Cell Encounter</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>2000000167</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Diagnoses</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Primary Diagnoses</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>2000000168</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Last Sickle Cell Encounter</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>2000000168</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Diagnoses</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>Primary Diagnoses</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>2000000169</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Adakveo</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>2000000169</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>2000000170</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Oxbrtya</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>2000000170</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>2000000171</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Voxeletor</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>2000000171</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>2000000172</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Hydroxyurea</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>2000000172</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
         <v>2000000173</v>
       </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Endari</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>2000000173</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>2000000174</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Deferasirox</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>2000000174</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>SCD Medication</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>2000000175</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Date of most recent transfusion of blood product</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>2000000175</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Transfusion</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>2000000176</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>2000000176</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Medication</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2000000177</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Primary Care Provider Name</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Common Registry</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>2000000177</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>2000000178</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Sickle Cell Diagnosis</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>2000000178</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Diagnoses</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Primary Diagnoses</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
handles concepts that are not questions.
</commit_message>
<xml_diff>
--- a/omop-questionconceptid-script/SCD_JobPackage.xlsx
+++ b/omop-questionconceptid-script/SCD_JobPackage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5714,6 +5714,306 @@
         </is>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2000000179</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>2000000179</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Lab Results</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Hepatobiliary</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2000000180</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Direct Bilirubin</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>2000000180</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Lab Results</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Hepatobiliary</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2000000181</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Lactate dehydrogenase</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>2000000181</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Lab Results</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Hepatobiliary</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2000000182</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Hemoglobin electrophoresis confirmation of disease.</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Special Code</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Class 1</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2000000183</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Likely has disease but no confirmation.</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Special Code</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Class 2</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2000000184</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Doubt of SCD but no confirmation of the negative assumption.</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Special Code</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Class 3</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2000000185</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Hemoglobin electrophoresis confirmed sickle cell trait.</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Special Code</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Class 9</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2000000186</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Does not have SCD=hbAA confirmed by electrophoresis.</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Special Code</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Class 0</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>2000000187</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Hemoglobin E Pct</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>2000000187</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Lab Results</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>Hemoglobin Electropheresis</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2000000188</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Classification Level</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>SCD Registry</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>2000000188</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Label</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>SCD Classification Level</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
registry jobpackage concept includes domain_id
</commit_message>
<xml_diff>
--- a/omop-questionconceptid-script/SCD_JobPackage.xlsx
+++ b/omop-questionconceptid-script/SCD_JobPackage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Domain_ID</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Question_Concept_Class</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Question_Concept_Code</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Section</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
@@ -489,15 +494,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>2000000001</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -518,15 +528,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>2000000002</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -547,15 +562,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>2000000003</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -576,15 +596,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
         <v>2000000004</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -605,15 +630,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>2000000005</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -634,15 +664,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>2000000006</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -663,15 +698,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>2000000025</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -692,15 +732,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>2000000026</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -721,15 +766,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>2000000027</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>Family History</t>
         </is>
@@ -754,15 +804,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>2000000028</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>Family History</t>
         </is>
@@ -787,15 +842,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>2000000029</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -820,15 +880,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>2000000030</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -853,15 +918,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>2000000031</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -886,15 +956,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>2000000032</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -919,15 +994,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>2000000033</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -952,15 +1032,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>2000000034</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -985,15 +1070,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
         <v>2000000035</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -1018,15 +1108,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>2000000036</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -1051,15 +1146,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>2000000037</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -1084,15 +1184,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
         <v>2000000038</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -1117,15 +1222,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>2000000039</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -1150,15 +1260,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>2000000040</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -1183,15 +1298,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
         <v>2000000041</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -1216,15 +1336,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
         <v>2000000042</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -1249,15 +1374,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
         <v>2000000043</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -1282,15 +1412,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
         <v>2000000044</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G27" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>Transplant</t>
         </is>
@@ -1315,15 +1450,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
         <v>2000000045</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>Transplant</t>
         </is>
@@ -1348,15 +1488,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
         <v>2000000046</v>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G29" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>Transplant</t>
         </is>
@@ -1381,15 +1526,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
         <v>2000000047</v>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G30" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1414,15 +1564,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
         <v>2000000048</v>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1447,15 +1602,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
         <v>2000000049</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1480,15 +1640,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
         <v>2000000050</v>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G33" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1513,15 +1678,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
         <v>2000000051</v>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1546,15 +1716,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
         <v>2000000052</v>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1579,15 +1754,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
         <v>2000000053</v>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G36" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1612,15 +1792,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
         <v>2000000054</v>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G37" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1645,15 +1830,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
         <v>2000000055</v>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G38" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1678,15 +1868,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
         <v>2000000056</v>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1711,15 +1906,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
         <v>2000000057</v>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G40" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -1744,15 +1944,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
         <v>2000000058</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1777,15 +1982,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
         <v>2000000059</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1810,15 +2020,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
         <v>2000000060</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1843,15 +2058,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
         <v>2000000061</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1876,15 +2096,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
         <v>2000000062</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1909,15 +2134,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
         <v>2000000063</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1942,15 +2172,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
         <v>2000000064</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -1975,15 +2210,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
         <v>2000000065</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -2008,15 +2248,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
         <v>2000000066</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -2041,15 +2286,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
         <v>2000000067</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2074,15 +2324,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E51" t="n">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
         <v>2000000068</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2107,15 +2362,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E52" t="n">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
         <v>2000000069</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2140,15 +2400,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E53" t="n">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
         <v>2000000070</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="G53" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2173,15 +2438,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E54" t="n">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
         <v>2000000071</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="G54" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="H54" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2206,15 +2476,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E55" t="n">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
         <v>2000000072</v>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="G55" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2239,15 +2514,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E56" t="n">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
         <v>2000000073</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="G56" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="H56" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2272,15 +2552,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E57" t="n">
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
         <v>2000000074</v>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="H57" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2305,15 +2590,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E58" t="n">
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
         <v>2000000075</v>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="G58" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="H58" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2338,15 +2628,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E59" t="n">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
         <v>2000000076</v>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="G59" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="H59" t="inlineStr">
         <is>
           <t>Blood Counts</t>
         </is>
@@ -2371,15 +2666,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E60" t="n">
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
         <v>2000000077</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="G60" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="H60" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2404,15 +2704,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E61" t="n">
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
         <v>2000000078</v>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="G61" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="H61" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2437,15 +2742,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E62" t="n">
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
         <v>2000000079</v>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="G62" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="H62" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2470,15 +2780,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E63" t="n">
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
         <v>2000000080</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="G63" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="H63" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2503,15 +2818,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E64" t="n">
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
         <v>2000000081</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="G64" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="H64" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2536,15 +2856,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E65" t="n">
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
         <v>2000000082</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="G65" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="H65" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2569,15 +2894,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E66" t="n">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
         <v>2000000083</v>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="G66" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="H66" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2602,15 +2932,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E67" t="n">
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
         <v>2000000084</v>
       </c>
-      <c r="F67" t="inlineStr">
+      <c r="G67" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="H67" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2635,15 +2970,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
         <v>2000000085</v>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="G68" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="H68" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2668,15 +3008,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E69" t="n">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
         <v>2000000086</v>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="G69" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr">
+      <c r="H69" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2701,15 +3046,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E70" t="n">
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
         <v>2000000087</v>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="G70" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="H70" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2734,15 +3084,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E71" t="n">
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
         <v>2000000088</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="G71" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="H71" t="inlineStr">
         <is>
           <t>Reticulocytes</t>
         </is>
@@ -2767,15 +3122,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E72" t="n">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
         <v>2000000089</v>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="G72" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="H72" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -2800,15 +3160,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E73" t="n">
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
         <v>2000000090</v>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="G73" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="H73" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -2833,15 +3198,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E74" t="n">
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
         <v>2000000091</v>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="G74" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="H74" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -2866,15 +3236,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E75" t="n">
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
         <v>2000000092</v>
       </c>
-      <c r="F75" t="inlineStr">
+      <c r="G75" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="H75" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -2899,15 +3274,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E76" t="n">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
         <v>2000000093</v>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G76" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -2932,15 +3312,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E77" t="n">
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
         <v>2000000094</v>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G77" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -2965,15 +3350,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E78" t="n">
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
         <v>2000000095</v>
       </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G78" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -2998,15 +3388,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E79" t="n">
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
         <v>2000000096</v>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G79" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3031,15 +3426,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E80" t="n">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
         <v>2000000097</v>
       </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G80" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3064,15 +3464,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E81" t="n">
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
         <v>2000000098</v>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G81" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3097,15 +3502,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E82" t="n">
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
         <v>2000000099</v>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G82" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3130,15 +3540,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E83" t="n">
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
         <v>2000000100</v>
       </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G83" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3163,15 +3578,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E84" t="n">
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
         <v>2000000101</v>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G84" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3196,15 +3616,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E85" t="n">
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
         <v>2000000102</v>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G85" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
         <is>
           <t>Renal</t>
         </is>
@@ -3229,15 +3654,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E86" t="n">
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
         <v>2000000103</v>
       </c>
-      <c r="F86" t="inlineStr">
+      <c r="G86" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="H86" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -3262,15 +3692,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E87" t="n">
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
         <v>2000000104</v>
       </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G87" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3295,15 +3730,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E88" t="n">
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
         <v>2000000105</v>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G88" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3328,15 +3768,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E89" t="n">
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
         <v>2000000106</v>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G89" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3361,15 +3806,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E90" t="n">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
         <v>2000000107</v>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G90" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3394,15 +3844,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E91" t="n">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
         <v>2000000108</v>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G91" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3427,15 +3882,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E92" t="n">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
         <v>2000000109</v>
       </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G92" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3460,15 +3920,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E93" t="n">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
         <v>2000000110</v>
       </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G93" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3493,15 +3958,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E94" t="n">
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
         <v>2000000111</v>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G94" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3526,15 +3996,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E95" t="n">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
         <v>2000000112</v>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G95" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3559,15 +4034,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E96" t="n">
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
         <v>2000000113</v>
       </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G96" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3592,15 +4072,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E97" t="n">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
         <v>2000000114</v>
       </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G97" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3625,15 +4110,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E98" t="n">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
         <v>2000000115</v>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G98" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3658,15 +4148,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E99" t="n">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
         <v>2000000116</v>
       </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G99" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3691,15 +4186,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E100" t="n">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
         <v>2000000117</v>
       </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G100" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
         <is>
           <t>Anemia</t>
         </is>
@@ -3724,15 +4224,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E101" t="n">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
         <v>2000000118</v>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G101" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3757,15 +4262,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E102" t="n">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
         <v>2000000119</v>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G102" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3790,15 +4300,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E103" t="n">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
         <v>2000000120</v>
       </c>
-      <c r="F103" t="inlineStr">
+      <c r="G103" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="H103" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -3823,15 +4338,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E104" t="n">
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
         <v>2000000121</v>
       </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G104" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -3856,15 +4376,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E105" t="n">
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
         <v>2000000122</v>
       </c>
-      <c r="F105" t="inlineStr">
+      <c r="G105" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="H105" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -3889,15 +4414,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E106" t="n">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
         <v>2000000123</v>
       </c>
-      <c r="F106" t="inlineStr">
+      <c r="G106" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
+      <c r="H106" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -3922,15 +4452,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E107" t="n">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
         <v>2000000124</v>
       </c>
-      <c r="F107" t="inlineStr">
+      <c r="G107" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
+      <c r="H107" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -3955,15 +4490,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E108" t="n">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
         <v>2000000125</v>
       </c>
-      <c r="F108" t="inlineStr">
+      <c r="G108" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
+      <c r="H108" t="inlineStr">
         <is>
           <t>Related Diagnoses</t>
         </is>
@@ -3988,15 +4528,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E109" t="n">
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
         <v>2000000126</v>
       </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G109" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4021,15 +4566,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E110" t="n">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
         <v>2000000127</v>
       </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G110" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4054,15 +4604,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E111" t="n">
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
         <v>2000000128</v>
       </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G111" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4087,15 +4642,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E112" t="n">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
         <v>2000000129</v>
       </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G112" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4120,15 +4680,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E113" t="n">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
         <v>2000000130</v>
       </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G113" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4153,15 +4718,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E114" t="n">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
         <v>2000000131</v>
       </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G114" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4186,15 +4756,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E115" t="n">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
         <v>2000000132</v>
       </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G115" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4219,15 +4794,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E116" t="n">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
         <v>2000000133</v>
       </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G116" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
         <is>
           <t>Pulmonary</t>
         </is>
@@ -4252,15 +4832,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E117" t="n">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
         <v>2000000134</v>
       </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G117" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
         <is>
           <t>General</t>
         </is>
@@ -4285,15 +4870,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E118" t="n">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
         <v>2000000135</v>
       </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G118" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
         <is>
           <t>General</t>
         </is>
@@ -4318,15 +4908,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E119" t="n">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
         <v>2000000136</v>
       </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G119" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4351,15 +4946,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E120" t="n">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
         <v>2000000137</v>
       </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G120" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4384,15 +4984,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E121" t="n">
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
         <v>2000000138</v>
       </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G121" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4417,15 +5022,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E122" t="n">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
         <v>2000000139</v>
       </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G122" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4450,15 +5060,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E123" t="n">
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
         <v>2000000140</v>
       </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G123" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4483,15 +5098,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E124" t="n">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
         <v>2000000141</v>
       </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G124" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4516,15 +5136,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E125" t="n">
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
         <v>2000000142</v>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G125" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4549,15 +5174,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E126" t="n">
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
         <v>2000000143</v>
       </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G126" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4582,15 +5212,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E127" t="n">
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
         <v>2000000144</v>
       </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G127" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4615,15 +5250,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E128" t="n">
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
         <v>2000000145</v>
       </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G128" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4648,15 +5288,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E129" t="n">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
         <v>2000000146</v>
       </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G129" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
         <is>
           <t>Cardiovascular</t>
         </is>
@@ -4681,15 +5326,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E130" t="n">
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
         <v>2000000147</v>
       </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G130" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
         <is>
           <t>General</t>
         </is>
@@ -4714,15 +5364,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E131" t="n">
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
         <v>2000000148</v>
       </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G131" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
         <is>
           <t>General</t>
         </is>
@@ -4747,15 +5402,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E132" t="n">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
         <v>2000000149</v>
       </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G132" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
         <is>
           <t>Neurological</t>
         </is>
@@ -4780,15 +5440,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E133" t="n">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
         <v>2000000150</v>
       </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G133" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
         <is>
           <t>Neurological</t>
         </is>
@@ -4813,15 +5478,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E134" t="n">
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
         <v>2000000151</v>
       </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G134" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
         <is>
           <t>Neurological</t>
         </is>
@@ -4846,15 +5516,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E135" t="n">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
         <v>2000000152</v>
       </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G135" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
         <is>
           <t>Neurological</t>
         </is>
@@ -4879,15 +5554,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E136" t="n">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
         <v>2000000153</v>
       </c>
-      <c r="F136" t="inlineStr">
+      <c r="G136" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G136" t="inlineStr">
+      <c r="H136" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -4912,15 +5592,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E137" t="n">
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
         <v>2000000154</v>
       </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G137" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
         <is>
           <t>Ophthalmological</t>
         </is>
@@ -4945,15 +5630,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E138" t="n">
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
         <v>2000000155</v>
       </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G138" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
         <is>
           <t>Ophthalmological</t>
         </is>
@@ -4978,15 +5668,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E139" t="n">
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
         <v>2000000156</v>
       </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G139" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
         <is>
           <t>Ophthalmological</t>
         </is>
@@ -5011,15 +5706,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E140" t="n">
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
         <v>2000000157</v>
       </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G140" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
         <is>
           <t>Ophthalmological</t>
         </is>
@@ -5044,15 +5744,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E141" t="n">
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
         <v>2000000158</v>
       </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G141" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
         <is>
           <t>Ophthalmological</t>
         </is>
@@ -5077,15 +5782,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E142" t="n">
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
         <v>2000000159</v>
       </c>
-      <c r="F142" t="inlineStr">
+      <c r="G142" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G142" t="inlineStr">
+      <c r="H142" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -5110,15 +5820,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E143" t="n">
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
         <v>2000000160</v>
       </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G143" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
         <is>
           <t>Orthopedic</t>
         </is>
@@ -5143,15 +5858,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E144" t="n">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
         <v>2000000161</v>
       </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G144" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
         <is>
           <t>Orthopedic</t>
         </is>
@@ -5176,15 +5896,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E145" t="n">
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
         <v>2000000162</v>
       </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G145" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
         <is>
           <t>Dermatological</t>
         </is>
@@ -5209,15 +5934,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E146" t="n">
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
         <v>2000000163</v>
       </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G146" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
         <is>
           <t>Dermatological</t>
         </is>
@@ -5242,15 +5972,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E147" t="n">
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
         <v>2000000164</v>
       </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G147" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
         <is>
           <t>General</t>
         </is>
@@ -5275,15 +6010,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E148" t="n">
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
         <v>2000000165</v>
       </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G148" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
         <is>
           <t>Urological</t>
         </is>
@@ -5308,15 +6048,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E149" t="n">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
         <v>2000000166</v>
       </c>
-      <c r="F149" t="inlineStr">
+      <c r="G149" t="inlineStr">
         <is>
           <t>Treatment</t>
         </is>
       </c>
-      <c r="G149" t="inlineStr">
+      <c r="H149" t="inlineStr">
         <is>
           <t>Primary Treatment</t>
         </is>
@@ -5341,15 +6086,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E150" t="n">
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
         <v>2000000167</v>
       </c>
-      <c r="F150" t="inlineStr">
+      <c r="G150" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G150" t="inlineStr">
+      <c r="H150" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -5374,15 +6124,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E151" t="n">
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
         <v>2000000168</v>
       </c>
-      <c r="F151" t="inlineStr">
+      <c r="G151" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G151" t="inlineStr">
+      <c r="H151" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -5407,15 +6162,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E152" t="n">
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
         <v>2000000169</v>
       </c>
-      <c r="F152" t="inlineStr">
+      <c r="G152" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G152" t="inlineStr">
+      <c r="H152" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5440,15 +6200,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E153" t="n">
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
         <v>2000000170</v>
       </c>
-      <c r="F153" t="inlineStr">
+      <c r="G153" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G153" t="inlineStr">
+      <c r="H153" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5473,15 +6238,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E154" t="n">
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
         <v>2000000171</v>
       </c>
-      <c r="F154" t="inlineStr">
+      <c r="G154" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G154" t="inlineStr">
+      <c r="H154" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5506,15 +6276,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E155" t="n">
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
         <v>2000000172</v>
       </c>
-      <c r="F155" t="inlineStr">
+      <c r="G155" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G155" t="inlineStr">
+      <c r="H155" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5539,15 +6314,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E156" t="n">
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
         <v>2000000173</v>
       </c>
-      <c r="F156" t="inlineStr">
+      <c r="G156" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G156" t="inlineStr">
+      <c r="H156" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5572,15 +6352,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E157" t="n">
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
         <v>2000000174</v>
       </c>
-      <c r="F157" t="inlineStr">
+      <c r="G157" t="inlineStr">
         <is>
           <t>SCD Medication</t>
         </is>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="H157" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5605,15 +6390,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E158" t="n">
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
         <v>2000000175</v>
       </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G158" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
         <is>
           <t>Transfusion</t>
         </is>
@@ -5638,15 +6428,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E159" t="n">
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
         <v>2000000176</v>
       </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>Other Medical History</t>
-        </is>
-      </c>
       <c r="G159" t="inlineStr">
+        <is>
+          <t>Other Medical History</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
         <is>
           <t>Medication</t>
         </is>
@@ -5671,15 +6466,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E160" t="n">
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F160" t="n">
         <v>2000000177</v>
       </c>
-      <c r="F160" t="inlineStr">
+      <c r="G160" t="inlineStr">
         <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -5700,15 +6500,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E161" t="n">
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
         <v>2000000178</v>
       </c>
-      <c r="F161" t="inlineStr">
+      <c r="G161" t="inlineStr">
         <is>
           <t>Diagnoses</t>
         </is>
       </c>
-      <c r="G161" t="inlineStr">
+      <c r="H161" t="inlineStr">
         <is>
           <t>Primary Diagnoses</t>
         </is>
@@ -5733,15 +6538,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E162" t="n">
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
         <v>2000000179</v>
       </c>
-      <c r="F162" t="inlineStr">
+      <c r="G162" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G162" t="inlineStr">
+      <c r="H162" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -5766,15 +6576,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E163" t="n">
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
         <v>2000000180</v>
       </c>
-      <c r="F163" t="inlineStr">
+      <c r="G163" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G163" t="inlineStr">
+      <c r="H163" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -5799,15 +6614,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E164" t="n">
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
         <v>2000000181</v>
       </c>
-      <c r="F164" t="inlineStr">
+      <c r="G164" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G164" t="inlineStr">
+      <c r="H164" t="inlineStr">
         <is>
           <t>Hepatobiliary</t>
         </is>
@@ -5829,16 +6649,21 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
+          <t>Meas Value</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
           <t>Special Code</t>
         </is>
       </c>
-      <c r="E165" t="inlineStr">
+      <c r="F165" t="inlineStr">
         <is>
           <t>Class 1</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr"/>
       <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -5856,16 +6681,21 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
+          <t>Meas Value</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
           <t>Special Code</t>
         </is>
       </c>
-      <c r="E166" t="inlineStr">
+      <c r="F166" t="inlineStr">
         <is>
           <t>Class 2</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr"/>
       <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -5883,16 +6713,21 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
+          <t>Meas Value</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
           <t>Special Code</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr">
+      <c r="F167" t="inlineStr">
         <is>
           <t>Class 3</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr"/>
       <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -5910,16 +6745,21 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
+          <t>Meas Value</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
           <t>Special Code</t>
         </is>
       </c>
-      <c r="E168" t="inlineStr">
+      <c r="F168" t="inlineStr">
         <is>
           <t>Class 9</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr"/>
       <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -5937,16 +6777,21 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
+          <t>Meas Value</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
           <t>Special Code</t>
         </is>
       </c>
-      <c r="E169" t="inlineStr">
+      <c r="F169" t="inlineStr">
         <is>
           <t>Class 0</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr"/>
       <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -5967,15 +6812,20 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="E170" t="n">
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
         <v>2000000187</v>
       </c>
-      <c r="F170" t="inlineStr">
+      <c r="G170" t="inlineStr">
         <is>
           <t>Lab Results</t>
         </is>
       </c>
-      <c r="G170" t="inlineStr">
+      <c r="H170" t="inlineStr">
         <is>
           <t>Hemoglobin Electropheresis</t>
         </is>
@@ -6000,15 +6850,20 @@
           <t>Measurement</t>
         </is>
       </c>
-      <c r="E171" t="n">
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="F171" t="n">
         <v>2000000188</v>
       </c>
-      <c r="F171" t="inlineStr">
+      <c r="G171" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="G171" t="inlineStr">
+      <c r="H171" t="inlineStr">
         <is>
           <t>SCD Classification Level</t>
         </is>

</xml_diff>